<commit_message>
update to latex document
</commit_message>
<xml_diff>
--- a/doc/sample results.xlsx
+++ b/doc/sample results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\honours\seirplus-dynamic-agents\result analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\honours\seirplus-dynamic-agents\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BE91609-D6F1-462B-B262-96E0683CA647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B80D98-06D5-4E5B-86B9-6A9D970E9509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3475D29E-48A1-4AD1-89AC-EF31B661C055}"/>
+    <workbookView xWindow="-9585" yWindow="2115" windowWidth="19275" windowHeight="12855" xr2:uid="{3475D29E-48A1-4AD1-89AC-EF31B661C055}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -133,8 +133,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1266,16 +1267,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1600,10 +1601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A146CD6-A580-4DBD-AA74-28A20C481967}">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1618,9 +1619,10 @@
     <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1640,7 +1642,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1662,8 +1664,15 @@
       <c r="L2" t="s">
         <v>19</v>
       </c>
+      <c r="N2" s="1"/>
+      <c r="O2">
+        <v>0.5</v>
+      </c>
+      <c r="P2">
+        <v>0.7</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1686,7 +1695,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1708,8 +1717,17 @@
       <c r="L4" t="s">
         <v>20</v>
       </c>
+      <c r="N4">
+        <v>0.4</v>
+      </c>
+      <c r="O4">
+        <v>0.6</v>
+      </c>
+      <c r="P4">
+        <v>0.8</v>
+      </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -1747,7 +1765,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>109</v>
       </c>
@@ -1785,7 +1803,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>191</v>
       </c>
@@ -1823,7 +1841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>107</v>
       </c>
@@ -1861,7 +1879,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>73</v>
       </c>
@@ -1899,7 +1917,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>96</v>
       </c>
@@ -1937,7 +1955,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>88</v>
       </c>
@@ -1975,7 +1993,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>92</v>
       </c>
@@ -2013,7 +2031,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>37</v>
       </c>
@@ -2051,7 +2069,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>56</v>
       </c>
@@ -2089,7 +2107,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>72</v>
       </c>

</xml_diff>